<commit_message>
MinJenV: inrichten op logische modellen conform MIM 1.2
MinJenV heeft tot nu toe alleen op SIM/UGM/BSM modellen gewerkt, maar
voor kennismaking met OpenAPI module van Armatiek is een MIM 1.2 model
nodig. Eerste stap is hiermee gezet.

Configuratie
</commit_message>
<xml_diff>
--- a/src/main/resources/input/MinJenV/props/MinJenV.xlsx
+++ b/src/main/resources/input/MinJenV/props/MinJenV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\MinJenV\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A40B469-336C-48D0-AF0D-ECC168EB53D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6B6DEE-9142-4F01-99C9-E8BC0537ABFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="2280" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MinJenV" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="361">
   <si>
     <t>Name</t>
   </si>
@@ -1100,6 +1100,15 @@
   </si>
   <si>
     <t>info@minJenV.nl</t>
+  </si>
+  <si>
+    <t>LOGICAL: uitgebreid</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>LOGICAL</t>
   </si>
 </sst>
 </file>
@@ -1704,14 +1713,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z158"/>
+  <dimension ref="A1:AC158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E64" sqref="E64"/>
       <selection pane="topRight" activeCell="E64" sqref="E64"/>
       <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
-      <selection pane="bottomRight" activeCell="E45" sqref="A45:XFD45"/>
+      <selection pane="bottomRight" activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1738,11 +1747,14 @@
     <col min="21" max="21" width="19.61328125" customWidth="1"/>
     <col min="22" max="23" width="18" customWidth="1"/>
     <col min="24" max="24" width="19.61328125" customWidth="1"/>
-    <col min="25" max="25" width="63.61328125" customWidth="1"/>
-    <col min="26" max="26" width="30.07421875" customWidth="1"/>
+    <col min="25" max="25" width="2.3828125" style="15" customWidth="1"/>
+    <col min="26" max="26" width="19.61328125" customWidth="1"/>
+    <col min="27" max="27" width="2.3828125" style="15" customWidth="1"/>
+    <col min="28" max="28" width="63.61328125" customWidth="1"/>
+    <col min="29" max="29" width="30.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="3" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:28" s="3" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1809,11 +1821,16 @@
       <c r="X1" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="3" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:28" s="3" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="31"/>
       <c r="G2" s="11"/>
       <c r="H2" s="2" t="s">
@@ -1863,8 +1880,13 @@
       <c r="X2" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" s="1" customFormat="1" ht="29.6" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="AA2" s="11"/>
+    </row>
+    <row r="3" spans="1:28" s="1" customFormat="1" ht="29.6" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>150</v>
       </c>
@@ -1884,8 +1906,10 @@
       <c r="G3" s="12"/>
       <c r="M3" s="12"/>
       <c r="S3" s="12"/>
-    </row>
-    <row r="4" spans="1:25" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y3" s="12"/>
+      <c r="AA3" s="12"/>
+    </row>
+    <row r="4" spans="1:28" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1907,8 +1931,10 @@
       <c r="G4" s="12"/>
       <c r="M4" s="12"/>
       <c r="S4" s="12"/>
-    </row>
-    <row r="5" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y4" s="12"/>
+      <c r="AA4" s="12"/>
+    </row>
+    <row r="5" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1930,8 +1956,10 @@
       <c r="G5" s="12"/>
       <c r="M5" s="12"/>
       <c r="S5" s="12"/>
-    </row>
-    <row r="6" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y5" s="12"/>
+      <c r="AA5" s="12"/>
+    </row>
+    <row r="6" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>153</v>
       </c>
@@ -1951,8 +1979,10 @@
       <c r="G6" s="12"/>
       <c r="M6" s="12"/>
       <c r="S6" s="12"/>
-    </row>
-    <row r="7" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y6" s="12"/>
+      <c r="AA6" s="12"/>
+    </row>
+    <row r="7" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="46" t="s">
         <v>9</v>
       </c>
@@ -1972,9 +2002,11 @@
       <c r="G7" s="12"/>
       <c r="M7" s="12"/>
       <c r="S7" s="12"/>
-      <c r="Y7" s="45"/>
-    </row>
-    <row r="8" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="45"/>
+    </row>
+    <row r="8" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="46"/>
       <c r="B8" s="46"/>
       <c r="C8" s="46"/>
@@ -1983,9 +2015,11 @@
       <c r="G8" s="12"/>
       <c r="M8" s="12"/>
       <c r="S8" s="12"/>
-      <c r="Y8" s="45"/>
-    </row>
-    <row r="9" spans="1:25" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="45"/>
+    </row>
+    <row r="9" spans="1:28" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>156</v>
       </c>
@@ -2007,9 +2041,11 @@
       <c r="G9" s="12"/>
       <c r="M9" s="12"/>
       <c r="S9" s="12"/>
-      <c r="Y9" s="21"/>
-    </row>
-    <row r="10" spans="1:25" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y9" s="12"/>
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="21"/>
+    </row>
+    <row r="10" spans="1:28" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -2031,8 +2067,10 @@
       <c r="G10" s="12"/>
       <c r="M10" s="12"/>
       <c r="S10" s="12"/>
-    </row>
-    <row r="11" spans="1:25" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y10" s="12"/>
+      <c r="AA10" s="12"/>
+    </row>
+    <row r="11" spans="1:28" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>158</v>
       </c>
@@ -2052,8 +2090,10 @@
       <c r="G11" s="12"/>
       <c r="M11" s="12"/>
       <c r="S11" s="12"/>
-    </row>
-    <row r="12" spans="1:25" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y11" s="12"/>
+      <c r="AA11" s="12"/>
+    </row>
+    <row r="12" spans="1:28" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>131</v>
       </c>
@@ -2073,8 +2113,10 @@
       <c r="G12" s="12"/>
       <c r="M12" s="12"/>
       <c r="S12" s="12"/>
-    </row>
-    <row r="13" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y12" s="12"/>
+      <c r="AA12" s="12"/>
+    </row>
+    <row r="13" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>234</v>
       </c>
@@ -2094,9 +2136,11 @@
       <c r="G13" s="12"/>
       <c r="M13" s="12"/>
       <c r="S13" s="12"/>
-      <c r="Y13" s="22"/>
-    </row>
-    <row r="14" spans="1:25" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y13" s="12"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="22"/>
+    </row>
+    <row r="14" spans="1:28" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2118,8 +2162,10 @@
       <c r="G14" s="12"/>
       <c r="M14" s="12"/>
       <c r="S14" s="12"/>
-    </row>
-    <row r="15" spans="1:25" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y14" s="12"/>
+      <c r="AA14" s="12"/>
+    </row>
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -2141,9 +2187,11 @@
       <c r="G15" s="12"/>
       <c r="M15" s="12"/>
       <c r="S15" s="12"/>
-      <c r="Y15" s="22"/>
-    </row>
-    <row r="16" spans="1:25" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y15" s="12"/>
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="22"/>
+    </row>
+    <row r="16" spans="1:28" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -2165,9 +2213,11 @@
       <c r="G16" s="12"/>
       <c r="M16" s="12"/>
       <c r="S16" s="12"/>
-      <c r="Y16" s="22"/>
-    </row>
-    <row r="17" spans="1:25" s="1" customFormat="1" ht="17.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y16" s="12"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="22"/>
+    </row>
+    <row r="17" spans="1:28" s="1" customFormat="1" ht="17.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>212</v>
       </c>
@@ -2189,8 +2239,10 @@
       <c r="G17" s="12"/>
       <c r="M17" s="12"/>
       <c r="S17" s="12"/>
-    </row>
-    <row r="18" spans="1:25" s="1" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y17" s="12"/>
+      <c r="AA17" s="12"/>
+    </row>
+    <row r="18" spans="1:28" s="1" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>214</v>
       </c>
@@ -2257,9 +2309,14 @@
       <c r="X18" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="Y18" s="22"/>
-    </row>
-    <row r="19" spans="1:25" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="AA18" s="12"/>
+      <c r="AB18" s="22"/>
+    </row>
+    <row r="19" spans="1:28" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>160</v>
       </c>
@@ -2281,8 +2338,10 @@
       <c r="G19" s="12"/>
       <c r="M19" s="12"/>
       <c r="S19" s="12"/>
-    </row>
-    <row r="20" spans="1:25" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y19" s="12"/>
+      <c r="AA19" s="12"/>
+    </row>
+    <row r="20" spans="1:28" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>133</v>
       </c>
@@ -2304,9 +2363,11 @@
       <c r="G20" s="12"/>
       <c r="M20" s="12"/>
       <c r="S20" s="12"/>
-      <c r="Y20" s="22"/>
-    </row>
-    <row r="21" spans="1:25" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y20" s="12"/>
+      <c r="AA20" s="12"/>
+      <c r="AB20" s="22"/>
+    </row>
+    <row r="21" spans="1:28" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>136</v>
       </c>
@@ -2328,9 +2389,11 @@
       <c r="G21" s="12"/>
       <c r="M21" s="12"/>
       <c r="S21" s="12"/>
-      <c r="Y21" s="22"/>
-    </row>
-    <row r="22" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y21" s="12"/>
+      <c r="AA21" s="12"/>
+      <c r="AB21" s="22"/>
+    </row>
+    <row r="22" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>139</v>
       </c>
@@ -2352,9 +2415,11 @@
       <c r="G22" s="12"/>
       <c r="M22" s="12"/>
       <c r="S22" s="12"/>
-      <c r="Y22" s="22"/>
-    </row>
-    <row r="23" spans="1:25" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y22" s="12"/>
+      <c r="AA22" s="12"/>
+      <c r="AB22" s="22"/>
+    </row>
+    <row r="23" spans="1:28" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A23" s="17" t="s">
         <v>25</v>
       </c>
@@ -2380,9 +2445,11 @@
       <c r="O23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="12"/>
-      <c r="Y23" s="21"/>
-    </row>
-    <row r="24" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y23" s="12"/>
+      <c r="AA23" s="12"/>
+      <c r="AB23" s="21"/>
+    </row>
+    <row r="24" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>162</v>
       </c>
@@ -2402,8 +2469,10 @@
       <c r="G24" s="12"/>
       <c r="M24" s="12"/>
       <c r="S24" s="12"/>
-    </row>
-    <row r="25" spans="1:25" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Y24" s="12"/>
+      <c r="AA24" s="12"/>
+    </row>
+    <row r="25" spans="1:28" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -2425,9 +2494,11 @@
       <c r="G25" s="12"/>
       <c r="M25" s="12"/>
       <c r="S25" s="12"/>
-      <c r="Y25" s="22"/>
-    </row>
-    <row r="26" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y25" s="12"/>
+      <c r="AA25" s="12"/>
+      <c r="AB25" s="22"/>
+    </row>
+    <row r="26" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -2467,9 +2538,14 @@
       <c r="X26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Y26" s="22"/>
-    </row>
-    <row r="27" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="22"/>
+    </row>
+    <row r="27" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>330</v>
       </c>
@@ -2509,9 +2585,14 @@
       <c r="X27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Y27" s="22"/>
-    </row>
-    <row r="28" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="22"/>
+    </row>
+    <row r="28" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -2533,9 +2614,11 @@
       <c r="G28" s="12"/>
       <c r="M28" s="12"/>
       <c r="S28" s="12"/>
-      <c r="Y28" s="22"/>
-    </row>
-    <row r="29" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y28" s="12"/>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="22"/>
+    </row>
+    <row r="29" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>141</v>
       </c>
@@ -2557,9 +2640,11 @@
       <c r="G29" s="12"/>
       <c r="M29" s="12"/>
       <c r="S29" s="12"/>
-      <c r="Y29" s="22"/>
-    </row>
-    <row r="30" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y29" s="12"/>
+      <c r="AA29" s="12"/>
+      <c r="AB29" s="22"/>
+    </row>
+    <row r="30" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>285</v>
       </c>
@@ -2579,9 +2664,11 @@
       <c r="G30" s="12"/>
       <c r="M30" s="12"/>
       <c r="S30" s="12"/>
-      <c r="Y30" s="22"/>
-    </row>
-    <row r="31" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y30" s="12"/>
+      <c r="AA30" s="12"/>
+      <c r="AB30" s="22"/>
+    </row>
+    <row r="31" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>247</v>
       </c>
@@ -2601,9 +2688,11 @@
       <c r="G31" s="12"/>
       <c r="M31" s="12"/>
       <c r="S31" s="12"/>
-      <c r="Y31" s="22"/>
-    </row>
-    <row r="32" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y31" s="12"/>
+      <c r="AA31" s="12"/>
+      <c r="AB31" s="22"/>
+    </row>
+    <row r="32" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>252</v>
       </c>
@@ -2627,9 +2716,12 @@
       <c r="S32" s="12"/>
       <c r="U32" s="19"/>
       <c r="X32" s="19"/>
-      <c r="Y32" s="22"/>
-    </row>
-    <row r="33" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y32" s="12"/>
+      <c r="Z32" s="19"/>
+      <c r="AA32" s="12"/>
+      <c r="AB32" s="22"/>
+    </row>
+    <row r="33" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -2663,9 +2755,11 @@
       </c>
       <c r="M33" s="12"/>
       <c r="S33" s="12"/>
-      <c r="Y33" s="22"/>
-    </row>
-    <row r="34" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y33" s="12"/>
+      <c r="AA33" s="12"/>
+      <c r="AB33" s="22"/>
+    </row>
+    <row r="34" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>164</v>
       </c>
@@ -2687,9 +2781,11 @@
       <c r="G34" s="12"/>
       <c r="M34" s="12"/>
       <c r="S34" s="12"/>
-      <c r="Y34" s="22"/>
-    </row>
-    <row r="35" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y34" s="12"/>
+      <c r="AA34" s="12"/>
+      <c r="AB34" s="22"/>
+    </row>
+    <row r="35" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>167</v>
       </c>
@@ -2711,9 +2807,11 @@
       <c r="G35" s="12"/>
       <c r="M35" s="12"/>
       <c r="S35" s="12"/>
-      <c r="Y35" s="22"/>
-    </row>
-    <row r="36" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y35" s="12"/>
+      <c r="AA35" s="12"/>
+      <c r="AB35" s="22"/>
+    </row>
+    <row r="36" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>257</v>
       </c>
@@ -2735,9 +2833,11 @@
       <c r="G36" s="12"/>
       <c r="M36" s="12"/>
       <c r="S36" s="12"/>
-      <c r="Y36" s="22"/>
-    </row>
-    <row r="37" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y36" s="12"/>
+      <c r="AA36" s="12"/>
+      <c r="AB36" s="22"/>
+    </row>
+    <row r="37" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="4" t="s">
         <v>37</v>
       </c>
@@ -2757,8 +2857,10 @@
       <c r="G37" s="12"/>
       <c r="M37" s="12"/>
       <c r="S37" s="12"/>
-    </row>
-    <row r="38" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y37" s="12"/>
+      <c r="AA37" s="12"/>
+    </row>
+    <row r="38" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
         <v>269</v>
       </c>
@@ -2779,10 +2881,12 @@
       <c r="H38" s="1"/>
       <c r="M38" s="18"/>
       <c r="S38" s="12"/>
-      <c r="Y38" s="21"/>
-      <c r="Z38" s="1"/>
-    </row>
-    <row r="39" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Y38" s="12"/>
+      <c r="AA38" s="12"/>
+      <c r="AB38" s="21"/>
+      <c r="AC38" s="1"/>
+    </row>
+    <row r="39" spans="1:29" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -2804,8 +2908,10 @@
       <c r="G39" s="12"/>
       <c r="M39" s="12"/>
       <c r="S39" s="12"/>
-    </row>
-    <row r="40" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y39" s="12"/>
+      <c r="AA39" s="12"/>
+    </row>
+    <row r="40" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -2827,9 +2933,11 @@
       <c r="G40" s="12"/>
       <c r="M40" s="12"/>
       <c r="S40" s="12"/>
-      <c r="Y40" s="22"/>
-    </row>
-    <row r="41" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y40" s="12"/>
+      <c r="AA40" s="12"/>
+      <c r="AB40" s="22"/>
+    </row>
+    <row r="41" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
@@ -2851,8 +2959,10 @@
       <c r="G41" s="12"/>
       <c r="M41" s="12"/>
       <c r="S41" s="12"/>
-    </row>
-    <row r="42" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y41" s="12"/>
+      <c r="AA41" s="12"/>
+    </row>
+    <row r="42" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A42" s="4" t="s">
         <v>251</v>
       </c>
@@ -2874,8 +2984,10 @@
       <c r="G42" s="12"/>
       <c r="M42" s="33"/>
       <c r="S42" s="33"/>
-    </row>
-    <row r="43" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y42" s="33"/>
+      <c r="AA42" s="33"/>
+    </row>
+    <row r="43" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
         <v>170</v>
       </c>
@@ -2909,9 +3021,14 @@
       <c r="X43" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Y43" s="22"/>
-    </row>
-    <row r="44" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y43" s="12"/>
+      <c r="Z43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA43" s="12"/>
+      <c r="AB43" s="22"/>
+    </row>
+    <row r="44" spans="1:29" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A44" s="17" t="s">
         <v>45</v>
       </c>
@@ -2944,9 +3061,12 @@
       <c r="V44" s="17"/>
       <c r="W44" s="17"/>
       <c r="X44" s="17"/>
-      <c r="Y44" s="21"/>
-    </row>
-    <row r="45" spans="1:26" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y44" s="12"/>
+      <c r="Z44" s="17"/>
+      <c r="AA44" s="12"/>
+      <c r="AB44" s="21"/>
+    </row>
+    <row r="45" spans="1:29" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="46" t="s">
         <v>47</v>
       </c>
@@ -2968,9 +3088,11 @@
       <c r="G45" s="12"/>
       <c r="M45" s="12"/>
       <c r="S45" s="12"/>
-      <c r="Y45" s="45"/>
-    </row>
-    <row r="46" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y45" s="12"/>
+      <c r="AA45" s="12"/>
+      <c r="AB45" s="45"/>
+    </row>
+    <row r="46" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A46" s="46"/>
       <c r="B46" s="46"/>
       <c r="C46" s="46"/>
@@ -2979,9 +3101,11 @@
       <c r="G46" s="12"/>
       <c r="M46" s="12"/>
       <c r="S46" s="12"/>
-      <c r="Y46" s="45"/>
-    </row>
-    <row r="47" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y46" s="12"/>
+      <c r="AA46" s="12"/>
+      <c r="AB46" s="45"/>
+    </row>
+    <row r="47" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>172</v>
       </c>
@@ -3001,8 +3125,10 @@
       <c r="G47" s="12"/>
       <c r="M47" s="12"/>
       <c r="S47" s="12"/>
-    </row>
-    <row r="48" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y47" s="12"/>
+      <c r="AA47" s="12"/>
+    </row>
+    <row r="48" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -3024,8 +3150,10 @@
       <c r="G48" s="12"/>
       <c r="M48" s="12"/>
       <c r="S48" s="12"/>
-    </row>
-    <row r="49" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y48" s="12"/>
+      <c r="AA48" s="12"/>
+    </row>
+    <row r="49" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A49" s="4" t="s">
         <v>51</v>
       </c>
@@ -3047,9 +3175,11 @@
       <c r="G49" s="40"/>
       <c r="M49" s="13"/>
       <c r="S49" s="12"/>
-      <c r="Y49" s="22"/>
-    </row>
-    <row r="50" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y49" s="12"/>
+      <c r="AA49" s="12"/>
+      <c r="AB49" s="22"/>
+    </row>
+    <row r="50" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>210</v>
       </c>
@@ -3071,10 +3201,12 @@
       <c r="G50" s="13"/>
       <c r="M50" s="12"/>
       <c r="S50" s="12"/>
-      <c r="Y50" s="22"/>
-      <c r="Z50"/>
-    </row>
-    <row r="51" spans="1:26" s="4" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y50" s="12"/>
+      <c r="AA50" s="12"/>
+      <c r="AB50" s="22"/>
+      <c r="AC50"/>
+    </row>
+    <row r="51" spans="1:29" s="4" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="17" t="s">
         <v>175</v>
       </c>
@@ -3096,9 +3228,11 @@
       <c r="G51" s="12"/>
       <c r="M51" s="12"/>
       <c r="S51" s="12"/>
-      <c r="Y51" s="21"/>
-    </row>
-    <row r="52" spans="1:26" s="4" customFormat="1" ht="86.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y51" s="12"/>
+      <c r="AA51" s="12"/>
+      <c r="AB51" s="21"/>
+    </row>
+    <row r="52" spans="1:29" s="4" customFormat="1" ht="86.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="17" t="s">
         <v>177</v>
       </c>
@@ -3130,9 +3264,12 @@
       <c r="X52" t="s">
         <v>316</v>
       </c>
-      <c r="Y52" s="21"/>
-    </row>
-    <row r="53" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y52" s="12"/>
+      <c r="Z52"/>
+      <c r="AA52" s="12"/>
+      <c r="AB52" s="21"/>
+    </row>
+    <row r="53" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="4" t="s">
         <v>54</v>
       </c>
@@ -3152,9 +3289,11 @@
       <c r="G53" s="36"/>
       <c r="M53" s="12"/>
       <c r="S53" s="12"/>
-      <c r="Y53" s="22"/>
-    </row>
-    <row r="54" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y53" s="12"/>
+      <c r="AA53" s="12"/>
+      <c r="AB53" s="22"/>
+    </row>
+    <row r="54" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="4" t="s">
         <v>56</v>
       </c>
@@ -3174,9 +3313,11 @@
       <c r="G54" s="36"/>
       <c r="M54" s="12"/>
       <c r="S54" s="12"/>
-      <c r="Y54" s="22"/>
-    </row>
-    <row r="55" spans="1:26" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y54" s="12"/>
+      <c r="AA54" s="12"/>
+      <c r="AB54" s="22"/>
+    </row>
+    <row r="55" spans="1:29" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="4" t="s">
         <v>58</v>
       </c>
@@ -3204,9 +3345,12 @@
       <c r="S55" s="12"/>
       <c r="U55" s="1"/>
       <c r="X55" s="1"/>
-      <c r="Y55" s="21"/>
-    </row>
-    <row r="56" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y55" s="12"/>
+      <c r="Z55" s="1"/>
+      <c r="AA55" s="12"/>
+      <c r="AB55" s="21"/>
+    </row>
+    <row r="56" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A56" s="4" t="s">
         <v>180</v>
       </c>
@@ -3226,9 +3370,11 @@
       <c r="G56" s="12"/>
       <c r="M56" s="12"/>
       <c r="S56" s="12"/>
-      <c r="Y56" s="22"/>
-    </row>
-    <row r="57" spans="1:26" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Y56" s="12"/>
+      <c r="AA56" s="12"/>
+      <c r="AB56" s="22"/>
+    </row>
+    <row r="57" spans="1:29" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A57" s="37" t="s">
         <v>275</v>
       </c>
@@ -3260,10 +3406,13 @@
       <c r="S57" s="12"/>
       <c r="U57" s="9"/>
       <c r="X57" s="9"/>
-      <c r="Y57" s="22"/>
-      <c r="Z57" s="1"/>
-    </row>
-    <row r="58" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y57" s="12"/>
+      <c r="Z57" s="9"/>
+      <c r="AA57" s="12"/>
+      <c r="AB57" s="22"/>
+      <c r="AC57" s="1"/>
+    </row>
+    <row r="58" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A58" s="4" t="s">
         <v>277</v>
       </c>
@@ -3283,10 +3432,12 @@
       <c r="G58" s="12"/>
       <c r="M58" s="12"/>
       <c r="S58" s="12"/>
-      <c r="Y58" s="22"/>
-      <c r="Z58" s="1"/>
-    </row>
-    <row r="59" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y58" s="12"/>
+      <c r="AA58" s="12"/>
+      <c r="AB58" s="22"/>
+      <c r="AC58" s="1"/>
+    </row>
+    <row r="59" spans="1:29" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A59" s="4" t="s">
         <v>182</v>
       </c>
@@ -3306,10 +3457,12 @@
       <c r="G59" s="12"/>
       <c r="M59" s="12"/>
       <c r="S59" s="12"/>
-      <c r="Y59" s="22"/>
-      <c r="Z59" s="1"/>
-    </row>
-    <row r="60" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y59" s="12"/>
+      <c r="AA59" s="12"/>
+      <c r="AB59" s="22"/>
+      <c r="AC59" s="1"/>
+    </row>
+    <row r="60" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="4" t="s">
         <v>280</v>
       </c>
@@ -3339,10 +3492,12 @@
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
       <c r="S60" s="12"/>
-      <c r="Y60" s="22"/>
-      <c r="Z60" s="1"/>
-    </row>
-    <row r="61" spans="1:26" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y60" s="12"/>
+      <c r="AA60" s="12"/>
+      <c r="AB60" s="22"/>
+      <c r="AC60" s="1"/>
+    </row>
+    <row r="61" spans="1:29" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="9" t="s">
         <v>230</v>
       </c>
@@ -3379,10 +3534,13 @@
       <c r="V61" s="9"/>
       <c r="W61" s="9"/>
       <c r="X61" s="9"/>
-      <c r="Y61" s="22"/>
-      <c r="Z61" s="1"/>
-    </row>
-    <row r="62" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y61" s="12"/>
+      <c r="Z61" s="9"/>
+      <c r="AA61" s="12"/>
+      <c r="AB61" s="22"/>
+      <c r="AC61" s="1"/>
+    </row>
+    <row r="62" spans="1:29" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A62" s="4" t="s">
         <v>184</v>
       </c>
@@ -3404,9 +3562,11 @@
       <c r="G62" s="12"/>
       <c r="M62" s="12"/>
       <c r="S62" s="12"/>
-      <c r="Y62" s="22"/>
-    </row>
-    <row r="63" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y62" s="12"/>
+      <c r="AA62" s="12"/>
+      <c r="AB62" s="22"/>
+    </row>
+    <row r="63" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A63" s="4" t="s">
         <v>60</v>
       </c>
@@ -3426,9 +3586,11 @@
       <c r="G63" s="12"/>
       <c r="M63" s="12"/>
       <c r="S63" s="12"/>
-      <c r="Y63" s="22"/>
-    </row>
-    <row r="64" spans="1:26" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Y63" s="12"/>
+      <c r="AA63" s="12"/>
+      <c r="AB63" s="22"/>
+    </row>
+    <row r="64" spans="1:29" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A64" s="4" t="s">
         <v>290</v>
       </c>
@@ -3450,10 +3612,12 @@
       <c r="G64" s="12"/>
       <c r="M64" s="12"/>
       <c r="S64" s="12"/>
-      <c r="Y64" s="22"/>
-      <c r="Z64" s="42"/>
-    </row>
-    <row r="65" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y64" s="12"/>
+      <c r="AA64" s="12"/>
+      <c r="AB64" s="22"/>
+      <c r="AC64" s="42"/>
+    </row>
+    <row r="65" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" s="4" t="s">
         <v>62</v>
       </c>
@@ -3475,9 +3639,11 @@
       <c r="G65" s="12"/>
       <c r="M65" s="12"/>
       <c r="S65" s="12"/>
-      <c r="Y65" s="22"/>
-    </row>
-    <row r="66" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y65" s="12"/>
+      <c r="AA65" s="12"/>
+      <c r="AB65" s="22"/>
+    </row>
+    <row r="66" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" s="4" t="s">
         <v>292</v>
       </c>
@@ -3494,9 +3660,11 @@
       <c r="G66" s="12"/>
       <c r="M66" s="12"/>
       <c r="S66" s="12"/>
-      <c r="Y66" s="22"/>
-    </row>
-    <row r="67" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y66" s="12"/>
+      <c r="AA66" s="12"/>
+      <c r="AB66" s="22"/>
+    </row>
+    <row r="67" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" s="37" t="s">
         <v>249</v>
       </c>
@@ -3516,9 +3684,11 @@
       <c r="G67" s="12"/>
       <c r="M67" s="12"/>
       <c r="S67" s="12"/>
-      <c r="Y67" s="22"/>
-    </row>
-    <row r="68" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y67" s="12"/>
+      <c r="AA67" s="12"/>
+      <c r="AB67" s="22"/>
+    </row>
+    <row r="68" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
         <v>65</v>
       </c>
@@ -3540,8 +3710,10 @@
       <c r="G68" s="12"/>
       <c r="M68" s="12"/>
       <c r="S68" s="12"/>
-    </row>
-    <row r="69" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y68" s="12"/>
+      <c r="AA68" s="12"/>
+    </row>
+    <row r="69" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
@@ -3563,8 +3735,10 @@
       <c r="G69" s="12"/>
       <c r="M69" s="12"/>
       <c r="S69" s="12"/>
-    </row>
-    <row r="70" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y69" s="12"/>
+      <c r="AA69" s="12"/>
+    </row>
+    <row r="70" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
         <v>241</v>
       </c>
@@ -3586,9 +3760,11 @@
       <c r="G70" s="12"/>
       <c r="M70" s="12"/>
       <c r="S70" s="12"/>
-      <c r="Y70" s="22"/>
-    </row>
-    <row r="71" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y70" s="12"/>
+      <c r="AA70" s="12"/>
+      <c r="AB70" s="22"/>
+    </row>
+    <row r="71" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
         <v>186</v>
       </c>
@@ -3610,9 +3786,11 @@
       <c r="G71" s="12"/>
       <c r="M71" s="12"/>
       <c r="S71" s="12"/>
-      <c r="Y71" s="22"/>
-    </row>
-    <row r="72" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y71" s="12"/>
+      <c r="AA71" s="12"/>
+      <c r="AB71" s="22"/>
+    </row>
+    <row r="72" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
@@ -3634,8 +3812,10 @@
       <c r="G72" s="12"/>
       <c r="M72" s="12"/>
       <c r="S72" s="12"/>
-    </row>
-    <row r="73" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y72" s="12"/>
+      <c r="AA72" s="12"/>
+    </row>
+    <row r="73" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
         <v>340</v>
       </c>
@@ -3700,8 +3880,13 @@
       <c r="X73" s="1" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="74" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y73" s="12"/>
+      <c r="Z73" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="AA73" s="12"/>
+    </row>
+    <row r="74" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>343</v>
       </c>
@@ -3766,8 +3951,13 @@
       <c r="X74" s="1" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="75" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y74" s="12"/>
+      <c r="Z74" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="AA74" s="12"/>
+    </row>
+    <row r="75" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
         <v>345</v>
       </c>
@@ -3832,8 +4022,13 @@
       <c r="X75" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="76" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y75" s="12"/>
+      <c r="Z75" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA75" s="12"/>
+    </row>
+    <row r="76" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
         <v>347</v>
       </c>
@@ -3854,8 +4049,10 @@
       <c r="M76" s="12"/>
       <c r="S76" s="12"/>
       <c r="T76"/>
-    </row>
-    <row r="77" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y76" s="12"/>
+      <c r="AA76" s="12"/>
+    </row>
+    <row r="77" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
         <v>189</v>
       </c>
@@ -3875,8 +4072,10 @@
       <c r="G77" s="12"/>
       <c r="M77" s="12"/>
       <c r="S77" s="12"/>
-    </row>
-    <row r="78" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y77" s="12"/>
+      <c r="AA77" s="12"/>
+    </row>
+    <row r="78" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A78" s="17" t="s">
         <v>71</v>
       </c>
@@ -3904,10 +4103,13 @@
       <c r="S78" s="12"/>
       <c r="U78" s="17"/>
       <c r="X78" s="17"/>
-      <c r="Y78" s="21"/>
-      <c r="Z78" s="43"/>
-    </row>
-    <row r="79" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y78" s="12"/>
+      <c r="Z78" s="17"/>
+      <c r="AA78" s="12"/>
+      <c r="AB78" s="21"/>
+      <c r="AC78" s="43"/>
+    </row>
+    <row r="79" spans="1:29" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="17" t="s">
         <v>333</v>
       </c>
@@ -3935,10 +4137,13 @@
       <c r="S79" s="12"/>
       <c r="U79" s="17"/>
       <c r="X79" s="17"/>
-      <c r="Y79" s="21"/>
-      <c r="Z79" s="43"/>
-    </row>
-    <row r="80" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y79" s="12"/>
+      <c r="Z79" s="17"/>
+      <c r="AA79" s="12"/>
+      <c r="AB79" s="21"/>
+      <c r="AC79" s="43"/>
+    </row>
+    <row r="80" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
         <v>208</v>
       </c>
@@ -3960,8 +4165,10 @@
       <c r="G80" s="12"/>
       <c r="M80" s="12"/>
       <c r="S80" s="12"/>
-    </row>
-    <row r="81" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y80" s="12"/>
+      <c r="AA80" s="12"/>
+    </row>
+    <row r="81" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
         <v>73</v>
       </c>
@@ -3989,8 +4196,11 @@
       <c r="S81" s="12"/>
       <c r="U81" s="17"/>
       <c r="X81" s="17"/>
-    </row>
-    <row r="82" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y81" s="12"/>
+      <c r="Z81" s="17"/>
+      <c r="AA81" s="12"/>
+    </row>
+    <row r="82" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
         <v>75</v>
       </c>
@@ -4012,8 +4222,10 @@
       <c r="G82" s="12"/>
       <c r="M82" s="12"/>
       <c r="S82" s="12"/>
-    </row>
-    <row r="83" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y82" s="12"/>
+      <c r="AA82" s="12"/>
+    </row>
+    <row r="83" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
         <v>77</v>
       </c>
@@ -4035,8 +4247,10 @@
       <c r="G83" s="12"/>
       <c r="M83" s="12"/>
       <c r="S83" s="12"/>
-    </row>
-    <row r="84" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y83" s="12"/>
+      <c r="AA83" s="12"/>
+    </row>
+    <row r="84" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A84" s="4" t="s">
         <v>80</v>
       </c>
@@ -4064,9 +4278,12 @@
       <c r="S84" s="12"/>
       <c r="U84" s="17"/>
       <c r="X84" s="17"/>
-      <c r="Y84" s="21"/>
-    </row>
-    <row r="85" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y84" s="12"/>
+      <c r="Z84" s="17"/>
+      <c r="AA84" s="12"/>
+      <c r="AB84" s="21"/>
+    </row>
+    <row r="85" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A85" s="4" t="s">
         <v>295</v>
       </c>
@@ -4084,9 +4301,11 @@
       <c r="H85" s="17"/>
       <c r="M85" s="12"/>
       <c r="S85" s="12"/>
-      <c r="Y85" s="22"/>
-    </row>
-    <row r="86" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y85" s="12"/>
+      <c r="AA85" s="12"/>
+      <c r="AB85" s="22"/>
+    </row>
+    <row r="86" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
         <v>190</v>
       </c>
@@ -4108,10 +4327,12 @@
       <c r="G86" s="12"/>
       <c r="M86" s="12"/>
       <c r="S86" s="12"/>
-      <c r="Y86" s="22"/>
-      <c r="Z86" s="4"/>
-    </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="Y86" s="12"/>
+      <c r="AA86" s="12"/>
+      <c r="AB86" s="22"/>
+      <c r="AC86" s="4"/>
+    </row>
+    <row r="87" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A87" s="4" t="s">
         <v>297</v>
       </c>
@@ -4129,10 +4350,12 @@
       <c r="G87" s="12"/>
       <c r="M87" s="12"/>
       <c r="S87" s="12"/>
-      <c r="Y87" s="22"/>
-      <c r="Z87" s="4"/>
-    </row>
-    <row r="88" spans="1:26" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y87" s="12"/>
+      <c r="AA87" s="12"/>
+      <c r="AB87" s="22"/>
+      <c r="AC87" s="4"/>
+    </row>
+    <row r="88" spans="1:29" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A88" s="4" t="s">
         <v>300</v>
       </c>
@@ -4150,10 +4373,12 @@
       <c r="G88" s="12"/>
       <c r="M88" s="12"/>
       <c r="S88" s="12"/>
-      <c r="Y88" s="22"/>
-      <c r="Z88" s="4"/>
-    </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="Y88" s="12"/>
+      <c r="AA88" s="12"/>
+      <c r="AB88" s="22"/>
+      <c r="AC88" s="4"/>
+    </row>
+    <row r="89" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A89" s="4" t="s">
         <v>303</v>
       </c>
@@ -4171,10 +4396,12 @@
       <c r="G89" s="12"/>
       <c r="M89" s="12"/>
       <c r="S89" s="12"/>
-      <c r="Y89" s="22"/>
-      <c r="Z89" s="4"/>
-    </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="Y89" s="12"/>
+      <c r="AA89" s="12"/>
+      <c r="AB89" s="22"/>
+      <c r="AC89" s="4"/>
+    </row>
+    <row r="90" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A90" s="4" t="s">
         <v>306</v>
       </c>
@@ -4192,10 +4419,12 @@
       <c r="G90" s="12"/>
       <c r="M90" s="12"/>
       <c r="S90" s="12"/>
-      <c r="Y90" s="22"/>
-      <c r="Z90" s="4"/>
-    </row>
-    <row r="91" spans="1:26" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Y90" s="12"/>
+      <c r="AA90" s="12"/>
+      <c r="AB90" s="22"/>
+      <c r="AC90" s="4"/>
+    </row>
+    <row r="91" spans="1:29" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A91" s="4" t="s">
         <v>193</v>
       </c>
@@ -4217,9 +4446,11 @@
       <c r="G91" s="12"/>
       <c r="M91" s="12"/>
       <c r="S91" s="12"/>
-      <c r="Y91" s="22"/>
-    </row>
-    <row r="92" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y91" s="12"/>
+      <c r="AA91" s="12"/>
+      <c r="AB91" s="22"/>
+    </row>
+    <row r="92" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
         <v>82</v>
       </c>
@@ -4286,9 +4517,14 @@
       <c r="X92" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="Y92" s="22"/>
-    </row>
-    <row r="93" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y92" s="12"/>
+      <c r="Z92" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA92" s="12"/>
+      <c r="AB92" s="22"/>
+    </row>
+    <row r="93" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="1" t="s">
         <v>84</v>
       </c>
@@ -4310,9 +4546,11 @@
       <c r="G93" s="12"/>
       <c r="M93" s="12"/>
       <c r="S93" s="12"/>
-      <c r="Y93" s="22"/>
-    </row>
-    <row r="94" spans="1:26" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y93" s="12"/>
+      <c r="AA93" s="12"/>
+      <c r="AB93" s="22"/>
+    </row>
+    <row r="94" spans="1:29" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A94" s="4" t="s">
         <v>88</v>
       </c>
@@ -4340,9 +4578,12 @@
       <c r="S94" s="12"/>
       <c r="U94" s="1"/>
       <c r="X94" s="1"/>
-      <c r="Y94" s="21"/>
-    </row>
-    <row r="95" spans="1:26" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y94" s="12"/>
+      <c r="Z94" s="1"/>
+      <c r="AA94" s="12"/>
+      <c r="AB94" s="21"/>
+    </row>
+    <row r="95" spans="1:29" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A95" s="4" t="s">
         <v>144</v>
       </c>
@@ -4364,9 +4605,11 @@
       <c r="G95" s="12"/>
       <c r="M95" s="12"/>
       <c r="S95" s="12"/>
-      <c r="Y95" s="22"/>
-    </row>
-    <row r="96" spans="1:26" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y95" s="12"/>
+      <c r="AA95" s="12"/>
+      <c r="AB95" s="22"/>
+    </row>
+    <row r="96" spans="1:29" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A96" s="17" t="s">
         <v>338</v>
       </c>
@@ -4397,9 +4640,11 @@
       <c r="X96" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Y96" s="22"/>
-    </row>
-    <row r="97" spans="1:26" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="Y96" s="12"/>
+      <c r="AA96" s="12"/>
+      <c r="AB96" s="22"/>
+    </row>
+    <row r="97" spans="1:29" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A97" s="1" t="s">
         <v>92</v>
       </c>
@@ -4421,8 +4666,10 @@
       <c r="G97" s="12"/>
       <c r="M97" s="12"/>
       <c r="S97" s="12"/>
-    </row>
-    <row r="98" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y97" s="12"/>
+      <c r="AA97" s="12"/>
+    </row>
+    <row r="98" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A98" s="32" t="s">
         <v>308</v>
       </c>
@@ -4441,9 +4688,11 @@
       <c r="G98" s="12"/>
       <c r="M98" s="12"/>
       <c r="S98" s="12"/>
-      <c r="Y98" s="22"/>
-    </row>
-    <row r="99" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y98" s="12"/>
+      <c r="AA98" s="12"/>
+      <c r="AB98" s="22"/>
+    </row>
+    <row r="99" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A99" s="32" t="s">
         <v>215</v>
       </c>
@@ -4465,9 +4714,11 @@
       <c r="G99" s="12"/>
       <c r="M99" s="12"/>
       <c r="S99" s="12"/>
-      <c r="Z99" s="43"/>
-    </row>
-    <row r="100" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y99" s="12"/>
+      <c r="AA99" s="12"/>
+      <c r="AC99" s="43"/>
+    </row>
+    <row r="100" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
         <v>146</v>
       </c>
@@ -4489,9 +4740,11 @@
       <c r="G100" s="12"/>
       <c r="M100" s="12"/>
       <c r="S100" s="12"/>
-      <c r="Y100" s="22"/>
-    </row>
-    <row r="101" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y100" s="12"/>
+      <c r="AA100" s="12"/>
+      <c r="AB100" s="22"/>
+    </row>
+    <row r="101" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
         <v>95</v>
       </c>
@@ -4513,9 +4766,11 @@
       <c r="G101" s="12"/>
       <c r="M101" s="12"/>
       <c r="S101" s="12"/>
-      <c r="Y101" s="22"/>
-    </row>
-    <row r="102" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y101" s="12"/>
+      <c r="AA101" s="12"/>
+      <c r="AB101" s="22"/>
+    </row>
+    <row r="102" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A102" s="4" t="s">
         <v>195</v>
       </c>
@@ -4537,9 +4792,11 @@
       <c r="G102" s="12"/>
       <c r="M102" s="12"/>
       <c r="S102" s="12"/>
-      <c r="Y102" s="22"/>
-    </row>
-    <row r="103" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y102" s="12"/>
+      <c r="AA102" s="12"/>
+      <c r="AB102" s="22"/>
+    </row>
+    <row r="103" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A103" s="4" t="s">
         <v>237</v>
       </c>
@@ -4559,9 +4816,11 @@
       <c r="G103" s="12"/>
       <c r="M103" s="12"/>
       <c r="S103" s="12"/>
-      <c r="Y103" s="22"/>
-    </row>
-    <row r="104" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y103" s="12"/>
+      <c r="AA103" s="12"/>
+      <c r="AB103" s="22"/>
+    </row>
+    <row r="104" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="4" t="s">
         <v>211</v>
       </c>
@@ -4583,9 +4842,11 @@
       <c r="G104" s="12"/>
       <c r="M104" s="12"/>
       <c r="S104" s="12"/>
-      <c r="Y104" s="22"/>
-    </row>
-    <row r="105" spans="1:26" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y104" s="12"/>
+      <c r="AA104" s="12"/>
+      <c r="AB104" s="22"/>
+    </row>
+    <row r="105" spans="1:29" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
         <v>97</v>
       </c>
@@ -4607,8 +4868,10 @@
       <c r="G105" s="12"/>
       <c r="M105" s="12"/>
       <c r="S105" s="12"/>
-    </row>
-    <row r="106" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y105" s="12"/>
+      <c r="AA105" s="12"/>
+    </row>
+    <row r="106" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="5" t="s">
         <v>271</v>
       </c>
@@ -4631,9 +4894,11 @@
       <c r="H106" s="1"/>
       <c r="M106" s="12"/>
       <c r="S106" s="12"/>
-      <c r="Z106" s="44"/>
-    </row>
-    <row r="107" spans="1:26" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y106" s="12"/>
+      <c r="AA106" s="12"/>
+      <c r="AC106" s="44"/>
+    </row>
+    <row r="107" spans="1:29" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
         <v>99</v>
       </c>
@@ -4655,10 +4920,12 @@
       <c r="G107" s="12"/>
       <c r="M107" s="12"/>
       <c r="S107" s="12"/>
-      <c r="Y107" s="22"/>
-      <c r="Z107" s="43"/>
-    </row>
-    <row r="108" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y107" s="12"/>
+      <c r="AA107" s="12"/>
+      <c r="AB107" s="22"/>
+      <c r="AC107" s="43"/>
+    </row>
+    <row r="108" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A108" s="33" t="s">
         <v>312</v>
       </c>
@@ -4680,10 +4947,12 @@
       <c r="G108" s="12"/>
       <c r="M108" s="12"/>
       <c r="S108" s="12"/>
-      <c r="Y108" s="22"/>
-      <c r="Z108" s="43"/>
-    </row>
-    <row r="109" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y108" s="12"/>
+      <c r="AA108" s="12"/>
+      <c r="AB108" s="22"/>
+      <c r="AC108" s="43"/>
+    </row>
+    <row r="109" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A109" s="1" t="s">
         <v>101</v>
       </c>
@@ -4705,8 +4974,10 @@
       <c r="G109" s="12"/>
       <c r="M109" s="12"/>
       <c r="S109" s="12"/>
-    </row>
-    <row r="110" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y109" s="12"/>
+      <c r="AA109" s="12"/>
+    </row>
+    <row r="110" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
         <v>198</v>
       </c>
@@ -4728,8 +4999,10 @@
       <c r="G110" s="12"/>
       <c r="M110" s="12"/>
       <c r="S110" s="12"/>
-    </row>
-    <row r="111" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y110" s="12"/>
+      <c r="AA110" s="12"/>
+    </row>
+    <row r="111" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A111" s="1" t="s">
         <v>103</v>
       </c>
@@ -4751,8 +5024,10 @@
       <c r="G111" s="12"/>
       <c r="M111" s="12"/>
       <c r="S111" s="12"/>
-    </row>
-    <row r="112" spans="1:26" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y111" s="12"/>
+      <c r="AA111" s="12"/>
+    </row>
+    <row r="112" spans="1:29" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A112" s="1" t="s">
         <v>107</v>
       </c>
@@ -4774,8 +5049,10 @@
       <c r="G112" s="12"/>
       <c r="M112" s="12"/>
       <c r="S112" s="12"/>
-    </row>
-    <row r="113" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y112" s="12"/>
+      <c r="AA112" s="12"/>
+    </row>
+    <row r="113" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="4" t="s">
         <v>109</v>
       </c>
@@ -4803,9 +5080,12 @@
       <c r="S113" s="12"/>
       <c r="U113" s="1"/>
       <c r="X113" s="1"/>
-      <c r="Y113" s="21"/>
-    </row>
-    <row r="114" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y113" s="12"/>
+      <c r="Z113" s="1"/>
+      <c r="AA113" s="12"/>
+      <c r="AB113" s="21"/>
+    </row>
+    <row r="114" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="4" t="s">
         <v>111</v>
       </c>
@@ -4828,9 +5108,11 @@
       <c r="H114" s="1"/>
       <c r="M114" s="12"/>
       <c r="S114" s="12"/>
-      <c r="Y114" s="21"/>
-    </row>
-    <row r="115" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y114" s="12"/>
+      <c r="AA114" s="12"/>
+      <c r="AB114" s="21"/>
+    </row>
+    <row r="115" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
         <v>113</v>
       </c>
@@ -4856,9 +5138,11 @@
       <c r="O115" s="1"/>
       <c r="R115" s="1"/>
       <c r="S115" s="12"/>
-      <c r="Y115" s="21"/>
-    </row>
-    <row r="116" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y115" s="12"/>
+      <c r="AA115" s="12"/>
+      <c r="AB115" s="21"/>
+    </row>
+    <row r="116" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A116" s="1" t="s">
         <v>115</v>
       </c>
@@ -4916,8 +5200,13 @@
       <c r="X116" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="117" spans="1:25" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y116" s="12"/>
+      <c r="Z116" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA116" s="12"/>
+    </row>
+    <row r="117" spans="1:28" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A117" s="32" t="s">
         <v>117</v>
       </c>
@@ -4975,8 +5264,13 @@
       <c r="X117" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="118" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y117" s="12"/>
+      <c r="Z117" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA117" s="12"/>
+    </row>
+    <row r="118" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A118" s="32" t="s">
         <v>118</v>
       </c>
@@ -5022,8 +5316,13 @@
       <c r="X118" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="119" spans="1:25" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y118" s="12"/>
+      <c r="Z118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA118" s="12"/>
+    </row>
+    <row r="119" spans="1:28" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A119" s="4" t="s">
         <v>148</v>
       </c>
@@ -5047,8 +5346,10 @@
       <c r="L119"/>
       <c r="M119" s="12"/>
       <c r="S119" s="12"/>
-    </row>
-    <row r="120" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y119" s="12"/>
+      <c r="AA119" s="12"/>
+    </row>
+    <row r="120" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A120" s="5" t="s">
         <v>273</v>
       </c>
@@ -5083,8 +5384,11 @@
       <c r="V120"/>
       <c r="W120"/>
       <c r="X120"/>
-    </row>
-    <row r="121" spans="1:25" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y120" s="12"/>
+      <c r="Z120"/>
+      <c r="AA120" s="12"/>
+    </row>
+    <row r="121" spans="1:28" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A121" s="23" t="s">
         <v>120</v>
       </c>
@@ -5144,8 +5448,11 @@
       <c r="X121" s="1" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="122" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y121" s="12"/>
+      <c r="Z121" s="1"/>
+      <c r="AA121" s="12"/>
+    </row>
+    <row r="122" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A122" s="32" t="s">
         <v>123</v>
       </c>
@@ -5203,8 +5510,13 @@
       <c r="X122" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="123" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y122" s="12"/>
+      <c r="Z122" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA122" s="12"/>
+    </row>
+    <row r="123" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A123" s="32" t="s">
         <v>229</v>
       </c>
@@ -5262,8 +5574,13 @@
       <c r="X123" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="124" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y123" s="12"/>
+      <c r="Z123" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA123" s="12"/>
+    </row>
+    <row r="124" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A124" s="32" t="s">
         <v>126</v>
       </c>
@@ -5285,8 +5602,10 @@
       <c r="G124" s="24"/>
       <c r="M124" s="12"/>
       <c r="S124" s="12"/>
-    </row>
-    <row r="125" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y124" s="12"/>
+      <c r="AA124" s="12"/>
+    </row>
+    <row r="125" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A125" s="1" t="s">
         <v>331</v>
       </c>
@@ -5305,8 +5624,10 @@
       <c r="G125" s="12"/>
       <c r="M125" s="12"/>
       <c r="S125" s="12"/>
-    </row>
-    <row r="126" spans="1:25" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="Y125" s="12"/>
+      <c r="AA125" s="12"/>
+    </row>
+    <row r="126" spans="1:28" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A126" s="32" t="s">
         <v>244</v>
       </c>
@@ -5328,9 +5649,11 @@
       <c r="G126" s="24"/>
       <c r="M126" s="12"/>
       <c r="S126" s="12"/>
-      <c r="Y126" s="22"/>
-    </row>
-    <row r="127" spans="1:25" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y126" s="12"/>
+      <c r="AA126" s="12"/>
+      <c r="AB126" s="22"/>
+    </row>
+    <row r="127" spans="1:28" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A127" s="32" t="s">
         <v>128</v>
       </c>
@@ -5352,9 +5675,11 @@
       <c r="G127" s="24"/>
       <c r="M127" s="12"/>
       <c r="S127" s="12"/>
-      <c r="Y127" s="22"/>
-    </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="Y127" s="12"/>
+      <c r="AA127" s="12"/>
+      <c r="AB127" s="22"/>
+    </row>
+    <row r="128" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A128" s="20"/>
       <c r="B128" s="20"/>
       <c r="C128" s="20"/>
@@ -5365,8 +5690,10 @@
       <c r="H128" s="19"/>
       <c r="N128" s="1"/>
       <c r="S128" s="12"/>
-    </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y128" s="12"/>
+      <c r="AA128" s="12"/>
+    </row>
+    <row r="129" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A129" s="20"/>
       <c r="B129" s="20"/>
       <c r="C129" s="20"/>
@@ -5376,8 +5703,10 @@
       <c r="G129" s="25"/>
       <c r="H129" s="19"/>
       <c r="S129" s="12"/>
-    </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y129" s="12"/>
+      <c r="AA129" s="12"/>
+    </row>
+    <row r="130" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A130" s="20"/>
       <c r="B130" s="20"/>
       <c r="C130" s="20"/>
@@ -5387,8 +5716,10 @@
       <c r="G130" s="25"/>
       <c r="H130" s="19"/>
       <c r="S130" s="12"/>
-    </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y130" s="12"/>
+      <c r="AA130" s="12"/>
+    </row>
+    <row r="131" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A131" s="20"/>
       <c r="B131" s="20"/>
       <c r="C131" s="20"/>
@@ -5398,8 +5729,10 @@
       <c r="G131" s="25"/>
       <c r="H131" s="19"/>
       <c r="S131" s="12"/>
-    </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y131" s="12"/>
+      <c r="AA131" s="12"/>
+    </row>
+    <row r="132" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A132" s="20"/>
       <c r="B132" s="20"/>
       <c r="C132" s="20"/>
@@ -5409,8 +5742,10 @@
       <c r="G132" s="25"/>
       <c r="H132" s="19"/>
       <c r="S132" s="12"/>
-    </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y132" s="12"/>
+      <c r="AA132" s="12"/>
+    </row>
+    <row r="133" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A133" s="20"/>
       <c r="B133" s="20"/>
       <c r="C133" s="20"/>
@@ -5420,8 +5755,10 @@
       <c r="G133" s="25"/>
       <c r="H133" s="19"/>
       <c r="S133" s="12"/>
-    </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y133" s="12"/>
+      <c r="AA133" s="12"/>
+    </row>
+    <row r="134" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A134" s="20"/>
       <c r="B134" s="20"/>
       <c r="C134" s="20"/>
@@ -5431,8 +5768,10 @@
       <c r="G134" s="25"/>
       <c r="H134" s="19"/>
       <c r="S134" s="12"/>
-    </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y134" s="12"/>
+      <c r="AA134" s="12"/>
+    </row>
+    <row r="135" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A135" s="20"/>
       <c r="B135" s="20"/>
       <c r="C135" s="20"/>
@@ -5442,8 +5781,10 @@
       <c r="G135" s="25"/>
       <c r="H135" s="19"/>
       <c r="S135" s="12"/>
-    </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y135" s="12"/>
+      <c r="AA135" s="12"/>
+    </row>
+    <row r="136" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A136" s="20"/>
       <c r="B136" s="20"/>
       <c r="C136" s="20"/>
@@ -5453,8 +5794,10 @@
       <c r="G136" s="25"/>
       <c r="H136" s="19"/>
       <c r="S136" s="12"/>
-    </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y136" s="12"/>
+      <c r="AA136" s="12"/>
+    </row>
+    <row r="137" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A137" s="20"/>
       <c r="B137" s="20"/>
       <c r="C137" s="20"/>
@@ -5463,8 +5806,10 @@
       <c r="F137" s="20"/>
       <c r="G137" s="25"/>
       <c r="S137" s="12"/>
-    </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y137" s="12"/>
+      <c r="AA137" s="12"/>
+    </row>
+    <row r="138" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A138" s="20"/>
       <c r="B138" s="20"/>
       <c r="C138" s="20"/>
@@ -5473,8 +5818,10 @@
       <c r="F138" s="20"/>
       <c r="G138" s="25"/>
       <c r="S138" s="12"/>
-    </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y138" s="12"/>
+      <c r="AA138" s="12"/>
+    </row>
+    <row r="139" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A139" s="20"/>
       <c r="B139" s="20"/>
       <c r="C139" s="20"/>
@@ -5483,8 +5830,10 @@
       <c r="F139" s="20"/>
       <c r="G139" s="25"/>
       <c r="S139" s="12"/>
-    </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y139" s="12"/>
+      <c r="AA139" s="12"/>
+    </row>
+    <row r="140" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A140" s="20"/>
       <c r="B140" s="20"/>
       <c r="C140" s="20"/>
@@ -5493,8 +5842,10 @@
       <c r="F140" s="20"/>
       <c r="G140" s="25"/>
       <c r="S140" s="12"/>
-    </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y140" s="12"/>
+      <c r="AA140" s="12"/>
+    </row>
+    <row r="141" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A141" s="20"/>
       <c r="B141" s="20"/>
       <c r="C141" s="20"/>
@@ -5503,8 +5854,10 @@
       <c r="F141" s="20"/>
       <c r="G141" s="25"/>
       <c r="S141" s="12"/>
-    </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y141" s="12"/>
+      <c r="AA141" s="12"/>
+    </row>
+    <row r="142" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A142" s="20"/>
       <c r="B142" s="20"/>
       <c r="C142" s="20"/>
@@ -5513,8 +5866,10 @@
       <c r="F142" s="20"/>
       <c r="G142" s="25"/>
       <c r="S142" s="12"/>
-    </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y142" s="12"/>
+      <c r="AA142" s="12"/>
+    </row>
+    <row r="143" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A143" s="20"/>
       <c r="B143" s="20"/>
       <c r="C143" s="20"/>
@@ -5523,8 +5878,10 @@
       <c r="F143" s="20"/>
       <c r="G143" s="25"/>
       <c r="S143" s="12"/>
-    </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y143" s="12"/>
+      <c r="AA143" s="12"/>
+    </row>
+    <row r="144" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A144" s="20"/>
       <c r="B144" s="20"/>
       <c r="C144" s="20"/>
@@ -5533,8 +5890,10 @@
       <c r="F144" s="20"/>
       <c r="G144" s="25"/>
       <c r="S144" s="12"/>
-    </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y144" s="12"/>
+      <c r="AA144" s="12"/>
+    </row>
+    <row r="145" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A145" s="20"/>
       <c r="B145" s="20"/>
       <c r="C145" s="20"/>
@@ -5543,8 +5902,10 @@
       <c r="F145" s="20"/>
       <c r="G145" s="25"/>
       <c r="S145" s="12"/>
-    </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y145" s="12"/>
+      <c r="AA145" s="12"/>
+    </row>
+    <row r="146" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A146" s="20"/>
       <c r="B146" s="20"/>
       <c r="C146" s="20"/>
@@ -5553,8 +5914,10 @@
       <c r="F146" s="20"/>
       <c r="G146" s="25"/>
       <c r="S146" s="12"/>
-    </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y146" s="12"/>
+      <c r="AA146" s="12"/>
+    </row>
+    <row r="147" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A147" s="20"/>
       <c r="B147" s="20"/>
       <c r="C147" s="20"/>
@@ -5563,8 +5926,10 @@
       <c r="F147" s="20"/>
       <c r="G147" s="25"/>
       <c r="S147" s="12"/>
-    </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y147" s="12"/>
+      <c r="AA147" s="12"/>
+    </row>
+    <row r="148" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A148" s="20"/>
       <c r="B148" s="20"/>
       <c r="C148" s="20"/>
@@ -5573,8 +5938,10 @@
       <c r="F148" s="20"/>
       <c r="G148" s="25"/>
       <c r="S148" s="12"/>
-    </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y148" s="12"/>
+      <c r="AA148" s="12"/>
+    </row>
+    <row r="149" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A149" s="20"/>
       <c r="B149" s="20"/>
       <c r="C149" s="20"/>
@@ -5583,8 +5950,10 @@
       <c r="F149" s="20"/>
       <c r="G149" s="25"/>
       <c r="S149" s="12"/>
-    </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y149" s="12"/>
+      <c r="AA149" s="12"/>
+    </row>
+    <row r="150" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A150" s="20"/>
       <c r="B150" s="20"/>
       <c r="C150" s="20"/>
@@ -5593,8 +5962,10 @@
       <c r="F150" s="20"/>
       <c r="G150" s="25"/>
       <c r="S150" s="12"/>
-    </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y150" s="12"/>
+      <c r="AA150" s="12"/>
+    </row>
+    <row r="151" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A151" s="20"/>
       <c r="B151" s="20"/>
       <c r="C151" s="20"/>
@@ -5603,8 +5974,10 @@
       <c r="F151" s="20"/>
       <c r="G151" s="25"/>
       <c r="S151" s="12"/>
-    </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y151" s="12"/>
+      <c r="AA151" s="12"/>
+    </row>
+    <row r="152" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A152" s="20"/>
       <c r="B152" s="20"/>
       <c r="C152" s="20"/>
@@ -5613,8 +5986,10 @@
       <c r="F152" s="20"/>
       <c r="G152" s="25"/>
       <c r="S152" s="12"/>
-    </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y152" s="12"/>
+      <c r="AA152" s="12"/>
+    </row>
+    <row r="153" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A153" s="20"/>
       <c r="B153" s="20"/>
       <c r="C153" s="20"/>
@@ -5623,8 +5998,10 @@
       <c r="F153" s="20"/>
       <c r="G153" s="25"/>
       <c r="S153" s="12"/>
-    </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y153" s="12"/>
+      <c r="AA153" s="12"/>
+    </row>
+    <row r="154" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A154" s="20"/>
       <c r="B154" s="20"/>
       <c r="C154" s="20"/>
@@ -5633,8 +6010,10 @@
       <c r="F154" s="20"/>
       <c r="G154" s="25"/>
       <c r="S154" s="12"/>
-    </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y154" s="12"/>
+      <c r="AA154" s="12"/>
+    </row>
+    <row r="155" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A155" s="20"/>
       <c r="B155" s="20"/>
       <c r="C155" s="20"/>
@@ -5643,8 +6022,10 @@
       <c r="F155" s="20"/>
       <c r="G155" s="25"/>
       <c r="S155" s="12"/>
-    </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y155" s="12"/>
+      <c r="AA155" s="12"/>
+    </row>
+    <row r="156" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A156" s="20"/>
       <c r="B156" s="20"/>
       <c r="C156" s="20"/>
@@ -5653,8 +6034,10 @@
       <c r="F156" s="20"/>
       <c r="G156" s="25"/>
       <c r="S156" s="12"/>
-    </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y156" s="12"/>
+      <c r="AA156" s="12"/>
+    </row>
+    <row r="157" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A157" s="20"/>
       <c r="B157" s="20"/>
       <c r="C157" s="20"/>
@@ -5663,8 +6046,10 @@
       <c r="F157" s="20"/>
       <c r="G157" s="25"/>
       <c r="S157" s="12"/>
-    </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="Y157" s="12"/>
+      <c r="AA157" s="12"/>
+    </row>
+    <row r="158" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A158" s="20"/>
       <c r="B158" s="20"/>
       <c r="C158" s="20"/>
@@ -5675,16 +6060,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="Y45:Y46"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="AB45:AB46"/>
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="C45:C46"/>
     <mergeCell ref="D45:D46"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>